<commit_message>
amended error handling by ungrouping summarised record counts in DSr, ISR and SMR functions
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_DSR_ISR_SMR.xlsx
+++ b/tests/testthat/testdata_DSR_ISR_SMR.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="719" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="719"/>
   </bookViews>
   <sheets>
-    <sheet name="testdata_multiarea_ref" sheetId="15" r:id="rId1"/>
-    <sheet name="testdata_multiarea" sheetId="5" r:id="rId2"/>
-    <sheet name="testdata_1976" sheetId="12" r:id="rId3"/>
-    <sheet name="refdata" sheetId="14" r:id="rId4"/>
-    <sheet name="testresults_ISR" sheetId="13" r:id="rId5"/>
-    <sheet name="testresults_DSR" sheetId="4" r:id="rId6"/>
-    <sheet name="testdata_err1" sheetId="7" r:id="rId7"/>
-    <sheet name="testdata_err2" sheetId="8" r:id="rId8"/>
-    <sheet name="testdata_err3" sheetId="9" r:id="rId9"/>
+    <sheet name="testdata_multigroup" sheetId="16" r:id="rId1"/>
+    <sheet name="testdata_multiarea_ref" sheetId="15" r:id="rId2"/>
+    <sheet name="testdata_multiarea" sheetId="5" r:id="rId3"/>
+    <sheet name="testdata_1976" sheetId="12" r:id="rId4"/>
+    <sheet name="refdata" sheetId="14" r:id="rId5"/>
+    <sheet name="testresults_ISR" sheetId="13" r:id="rId6"/>
+    <sheet name="testresults_DSR" sheetId="4" r:id="rId7"/>
+    <sheet name="testdata_err1" sheetId="7" r:id="rId8"/>
+    <sheet name="testdata_err2" sheetId="8" r:id="rId9"/>
+    <sheet name="testdata_err3" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="58">
   <si>
     <t>0-4</t>
   </si>
@@ -203,6 +204,9 @@
   </si>
   <si>
     <t>smr x 100</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -647,6 +651,2291 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E115"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>2015</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>127</v>
+      </c>
+      <c r="E2">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>2015</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
+      <c r="E3">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
+        <v>2015</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>2015</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>21</v>
+      </c>
+      <c r="E5">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>2015</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>2015</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>27</v>
+      </c>
+      <c r="E7">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>2015</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>48</v>
+      </c>
+      <c r="E8">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>2015</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>27</v>
+      </c>
+      <c r="E9">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>2015</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>29</v>
+      </c>
+      <c r="E10">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>2015</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>32</v>
+      </c>
+      <c r="E11">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>2015</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>32</v>
+      </c>
+      <c r="E12">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13">
+        <v>2015</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>34</v>
+      </c>
+      <c r="E13">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>2015</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>45</v>
+      </c>
+      <c r="E14">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>2015</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>65</v>
+      </c>
+      <c r="E15">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>2015</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>38</v>
+      </c>
+      <c r="E16">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>2015</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>68</v>
+      </c>
+      <c r="E17">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>2015</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <v>74</v>
+      </c>
+      <c r="E18">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>2015</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <v>82</v>
+      </c>
+      <c r="E19">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>2015</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20">
+        <v>91</v>
+      </c>
+      <c r="E20">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>2015</v>
+      </c>
+      <c r="C21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>12</v>
+      </c>
+      <c r="E21">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>2015</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>2015</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>2015</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>2015</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>2015</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <v>4</v>
+      </c>
+      <c r="E26">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>2015</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28">
+        <v>2015</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <v>2015</v>
+      </c>
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30">
+        <v>2015</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31">
+        <v>2015</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>4</v>
+      </c>
+      <c r="E31">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32">
+        <v>2015</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
+      <c r="E32">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33">
+        <v>2015</v>
+      </c>
+      <c r="C33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33">
+        <v>6</v>
+      </c>
+      <c r="E33">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34">
+        <v>2015</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34">
+        <v>8</v>
+      </c>
+      <c r="E34">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35">
+        <v>2015</v>
+      </c>
+      <c r="C35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+      <c r="E35">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36">
+        <v>2015</v>
+      </c>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36">
+        <v>6</v>
+      </c>
+      <c r="E36">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37">
+        <v>2015</v>
+      </c>
+      <c r="C37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+      <c r="E37">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38">
+        <v>2015</v>
+      </c>
+      <c r="C38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
+      <c r="E38">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39">
+        <v>2015</v>
+      </c>
+      <c r="C39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="E39">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40">
+        <v>2015</v>
+      </c>
+      <c r="C40" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41">
+        <v>2015</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42">
+        <v>2015</v>
+      </c>
+      <c r="C42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43">
+        <v>2015</v>
+      </c>
+      <c r="C43" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44">
+        <v>2015</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>29</v>
+      </c>
+      <c r="B45">
+        <v>2015</v>
+      </c>
+      <c r="C45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>29</v>
+      </c>
+      <c r="B46">
+        <v>2015</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>29</v>
+      </c>
+      <c r="B47">
+        <v>2015</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48">
+        <v>2015</v>
+      </c>
+      <c r="C48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49">
+        <v>2015</v>
+      </c>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>29</v>
+      </c>
+      <c r="B50">
+        <v>2015</v>
+      </c>
+      <c r="C50" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>29</v>
+      </c>
+      <c r="B51">
+        <v>2015</v>
+      </c>
+      <c r="C51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>29</v>
+      </c>
+      <c r="B52">
+        <v>2015</v>
+      </c>
+      <c r="C52" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>29</v>
+      </c>
+      <c r="B53">
+        <v>2015</v>
+      </c>
+      <c r="C53" t="s">
+        <v>13</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>29</v>
+      </c>
+      <c r="B54">
+        <v>2015</v>
+      </c>
+      <c r="C54" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>29</v>
+      </c>
+      <c r="B55">
+        <v>2015</v>
+      </c>
+      <c r="C55" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56">
+        <v>2015</v>
+      </c>
+      <c r="C56" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>29</v>
+      </c>
+      <c r="B57">
+        <v>2015</v>
+      </c>
+      <c r="C57" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>29</v>
+      </c>
+      <c r="B58">
+        <v>2015</v>
+      </c>
+      <c r="C58" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58">
+        <v>3</v>
+      </c>
+      <c r="E58">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>23</v>
+      </c>
+      <c r="B59">
+        <v>2016</v>
+      </c>
+      <c r="C59" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>137</v>
+      </c>
+      <c r="E59">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>23</v>
+      </c>
+      <c r="B60">
+        <v>2016</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>35</v>
+      </c>
+      <c r="E60">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>23</v>
+      </c>
+      <c r="B61">
+        <v>2016</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61">
+        <v>28</v>
+      </c>
+      <c r="E61">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>23</v>
+      </c>
+      <c r="B62">
+        <v>2016</v>
+      </c>
+      <c r="C62" t="s">
+        <v>3</v>
+      </c>
+      <c r="D62">
+        <v>31</v>
+      </c>
+      <c r="E62">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>23</v>
+      </c>
+      <c r="B63">
+        <v>2016</v>
+      </c>
+      <c r="C63" t="s">
+        <v>4</v>
+      </c>
+      <c r="D63">
+        <v>22</v>
+      </c>
+      <c r="E63">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>23</v>
+      </c>
+      <c r="B64">
+        <v>2016</v>
+      </c>
+      <c r="C64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64">
+        <v>37</v>
+      </c>
+      <c r="E64">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>23</v>
+      </c>
+      <c r="B65">
+        <v>2016</v>
+      </c>
+      <c r="C65" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65">
+        <v>58</v>
+      </c>
+      <c r="E65">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>23</v>
+      </c>
+      <c r="B66">
+        <v>2016</v>
+      </c>
+      <c r="C66" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66">
+        <v>37</v>
+      </c>
+      <c r="E66">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>23</v>
+      </c>
+      <c r="B67">
+        <v>2016</v>
+      </c>
+      <c r="C67" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67">
+        <v>39</v>
+      </c>
+      <c r="E67">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>23</v>
+      </c>
+      <c r="B68">
+        <v>2016</v>
+      </c>
+      <c r="C68" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68">
+        <v>42</v>
+      </c>
+      <c r="E68">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>23</v>
+      </c>
+      <c r="B69">
+        <v>2016</v>
+      </c>
+      <c r="C69" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69">
+        <v>42</v>
+      </c>
+      <c r="E69">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>23</v>
+      </c>
+      <c r="B70">
+        <v>2016</v>
+      </c>
+      <c r="C70" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70">
+        <v>44</v>
+      </c>
+      <c r="E70">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>23</v>
+      </c>
+      <c r="B71">
+        <v>2016</v>
+      </c>
+      <c r="C71" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71">
+        <v>55</v>
+      </c>
+      <c r="E71">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>23</v>
+      </c>
+      <c r="B72">
+        <v>2016</v>
+      </c>
+      <c r="C72" t="s">
+        <v>13</v>
+      </c>
+      <c r="D72">
+        <v>75</v>
+      </c>
+      <c r="E72">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>23</v>
+      </c>
+      <c r="B73">
+        <v>2016</v>
+      </c>
+      <c r="C73" t="s">
+        <v>14</v>
+      </c>
+      <c r="D73">
+        <v>48</v>
+      </c>
+      <c r="E73">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>23</v>
+      </c>
+      <c r="B74">
+        <v>2016</v>
+      </c>
+      <c r="C74" t="s">
+        <v>15</v>
+      </c>
+      <c r="D74">
+        <v>78</v>
+      </c>
+      <c r="E74">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>23</v>
+      </c>
+      <c r="B75">
+        <v>2016</v>
+      </c>
+      <c r="C75" t="s">
+        <v>16</v>
+      </c>
+      <c r="D75">
+        <v>84</v>
+      </c>
+      <c r="E75">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>23</v>
+      </c>
+      <c r="B76">
+        <v>2016</v>
+      </c>
+      <c r="C76" t="s">
+        <v>17</v>
+      </c>
+      <c r="D76">
+        <v>92</v>
+      </c>
+      <c r="E76">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>23</v>
+      </c>
+      <c r="B77">
+        <v>2016</v>
+      </c>
+      <c r="C77" t="s">
+        <v>18</v>
+      </c>
+      <c r="D77">
+        <v>101</v>
+      </c>
+      <c r="E77">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>24</v>
+      </c>
+      <c r="B78">
+        <v>2016</v>
+      </c>
+      <c r="C78" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>22</v>
+      </c>
+      <c r="E78">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>24</v>
+      </c>
+      <c r="B79">
+        <v>2016</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>14</v>
+      </c>
+      <c r="E79">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>24</v>
+      </c>
+      <c r="B80">
+        <v>2016</v>
+      </c>
+      <c r="C80" t="s">
+        <v>2</v>
+      </c>
+      <c r="D80">
+        <v>13</v>
+      </c>
+      <c r="E80">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>24</v>
+      </c>
+      <c r="B81">
+        <v>2016</v>
+      </c>
+      <c r="C81" t="s">
+        <v>3</v>
+      </c>
+      <c r="D81">
+        <v>12</v>
+      </c>
+      <c r="E81">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>24</v>
+      </c>
+      <c r="B82">
+        <v>2016</v>
+      </c>
+      <c r="C82" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82">
+        <v>13</v>
+      </c>
+      <c r="E82">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>24</v>
+      </c>
+      <c r="B83">
+        <v>2016</v>
+      </c>
+      <c r="C83" t="s">
+        <v>5</v>
+      </c>
+      <c r="D83">
+        <v>14</v>
+      </c>
+      <c r="E83">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>24</v>
+      </c>
+      <c r="B84">
+        <v>2016</v>
+      </c>
+      <c r="C84" t="s">
+        <v>6</v>
+      </c>
+      <c r="D84">
+        <v>18</v>
+      </c>
+      <c r="E84">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>24</v>
+      </c>
+      <c r="B85">
+        <v>2016</v>
+      </c>
+      <c r="C85" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85">
+        <v>12</v>
+      </c>
+      <c r="E85">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>24</v>
+      </c>
+      <c r="B86">
+        <v>2016</v>
+      </c>
+      <c r="C86" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86">
+        <v>12</v>
+      </c>
+      <c r="E86">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>24</v>
+      </c>
+      <c r="B87">
+        <v>2016</v>
+      </c>
+      <c r="C87" t="s">
+        <v>9</v>
+      </c>
+      <c r="D87">
+        <v>13</v>
+      </c>
+      <c r="E87">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>24</v>
+      </c>
+      <c r="B88">
+        <v>2016</v>
+      </c>
+      <c r="C88" t="s">
+        <v>10</v>
+      </c>
+      <c r="D88">
+        <v>14</v>
+      </c>
+      <c r="E88">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>24</v>
+      </c>
+      <c r="B89">
+        <v>2016</v>
+      </c>
+      <c r="C89" t="s">
+        <v>11</v>
+      </c>
+      <c r="D89">
+        <v>15</v>
+      </c>
+      <c r="E89">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>24</v>
+      </c>
+      <c r="B90">
+        <v>2016</v>
+      </c>
+      <c r="C90" t="s">
+        <v>12</v>
+      </c>
+      <c r="D90">
+        <v>16</v>
+      </c>
+      <c r="E90">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>24</v>
+      </c>
+      <c r="B91">
+        <v>2016</v>
+      </c>
+      <c r="C91" t="s">
+        <v>13</v>
+      </c>
+      <c r="D91">
+        <v>18</v>
+      </c>
+      <c r="E91">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>24</v>
+      </c>
+      <c r="B92">
+        <v>2016</v>
+      </c>
+      <c r="C92" t="s">
+        <v>14</v>
+      </c>
+      <c r="D92">
+        <v>15</v>
+      </c>
+      <c r="E92">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>24</v>
+      </c>
+      <c r="B93">
+        <v>2016</v>
+      </c>
+      <c r="C93" t="s">
+        <v>15</v>
+      </c>
+      <c r="D93">
+        <v>16</v>
+      </c>
+      <c r="E93">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>24</v>
+      </c>
+      <c r="B94">
+        <v>2016</v>
+      </c>
+      <c r="C94" t="s">
+        <v>16</v>
+      </c>
+      <c r="D94">
+        <v>15</v>
+      </c>
+      <c r="E94">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>24</v>
+      </c>
+      <c r="B95">
+        <v>2016</v>
+      </c>
+      <c r="C95" t="s">
+        <v>17</v>
+      </c>
+      <c r="D95">
+        <v>15</v>
+      </c>
+      <c r="E95">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>24</v>
+      </c>
+      <c r="B96">
+        <v>2016</v>
+      </c>
+      <c r="C96" t="s">
+        <v>18</v>
+      </c>
+      <c r="D96">
+        <v>14</v>
+      </c>
+      <c r="E96">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>29</v>
+      </c>
+      <c r="B97">
+        <v>2016</v>
+      </c>
+      <c r="C97" t="s">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>10</v>
+      </c>
+      <c r="E97">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>29</v>
+      </c>
+      <c r="B98">
+        <v>2016</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <v>10</v>
+      </c>
+      <c r="E98">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>29</v>
+      </c>
+      <c r="B99">
+        <v>2016</v>
+      </c>
+      <c r="C99" t="s">
+        <v>2</v>
+      </c>
+      <c r="D99">
+        <v>10</v>
+      </c>
+      <c r="E99">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>29</v>
+      </c>
+      <c r="B100">
+        <v>2016</v>
+      </c>
+      <c r="C100" t="s">
+        <v>3</v>
+      </c>
+      <c r="D100">
+        <v>10</v>
+      </c>
+      <c r="E100">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>29</v>
+      </c>
+      <c r="B101">
+        <v>2016</v>
+      </c>
+      <c r="C101" t="s">
+        <v>4</v>
+      </c>
+      <c r="D101">
+        <v>10</v>
+      </c>
+      <c r="E101">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>29</v>
+      </c>
+      <c r="B102">
+        <v>2016</v>
+      </c>
+      <c r="C102" t="s">
+        <v>5</v>
+      </c>
+      <c r="D102">
+        <v>10</v>
+      </c>
+      <c r="E102">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>29</v>
+      </c>
+      <c r="B103">
+        <v>2016</v>
+      </c>
+      <c r="C103" t="s">
+        <v>6</v>
+      </c>
+      <c r="D103">
+        <v>11</v>
+      </c>
+      <c r="E103">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>29</v>
+      </c>
+      <c r="B104">
+        <v>2016</v>
+      </c>
+      <c r="C104" t="s">
+        <v>7</v>
+      </c>
+      <c r="D104">
+        <v>10</v>
+      </c>
+      <c r="E104">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>29</v>
+      </c>
+      <c r="B105">
+        <v>2016</v>
+      </c>
+      <c r="C105" t="s">
+        <v>8</v>
+      </c>
+      <c r="D105">
+        <v>10</v>
+      </c>
+      <c r="E105">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>29</v>
+      </c>
+      <c r="B106">
+        <v>2016</v>
+      </c>
+      <c r="C106" t="s">
+        <v>9</v>
+      </c>
+      <c r="D106">
+        <v>10</v>
+      </c>
+      <c r="E106">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>29</v>
+      </c>
+      <c r="B107">
+        <v>2016</v>
+      </c>
+      <c r="C107" t="s">
+        <v>10</v>
+      </c>
+      <c r="D107">
+        <v>10</v>
+      </c>
+      <c r="E107">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>29</v>
+      </c>
+      <c r="B108">
+        <v>2016</v>
+      </c>
+      <c r="C108" t="s">
+        <v>11</v>
+      </c>
+      <c r="D108">
+        <v>10</v>
+      </c>
+      <c r="E108">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>29</v>
+      </c>
+      <c r="B109">
+        <v>2016</v>
+      </c>
+      <c r="C109" t="s">
+        <v>12</v>
+      </c>
+      <c r="D109">
+        <v>11</v>
+      </c>
+      <c r="E109">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>29</v>
+      </c>
+      <c r="B110">
+        <v>2016</v>
+      </c>
+      <c r="C110" t="s">
+        <v>13</v>
+      </c>
+      <c r="D110">
+        <v>10</v>
+      </c>
+      <c r="E110">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>29</v>
+      </c>
+      <c r="B111">
+        <v>2016</v>
+      </c>
+      <c r="C111" t="s">
+        <v>14</v>
+      </c>
+      <c r="D111">
+        <v>10</v>
+      </c>
+      <c r="E111">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>29</v>
+      </c>
+      <c r="B112">
+        <v>2016</v>
+      </c>
+      <c r="C112" t="s">
+        <v>15</v>
+      </c>
+      <c r="D112">
+        <v>11</v>
+      </c>
+      <c r="E112">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>29</v>
+      </c>
+      <c r="B113">
+        <v>2016</v>
+      </c>
+      <c r="C113" t="s">
+        <v>16</v>
+      </c>
+      <c r="D113">
+        <v>11</v>
+      </c>
+      <c r="E113">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>29</v>
+      </c>
+      <c r="B114">
+        <v>2016</v>
+      </c>
+      <c r="C114" t="s">
+        <v>17</v>
+      </c>
+      <c r="D114">
+        <v>12</v>
+      </c>
+      <c r="E114">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>29</v>
+      </c>
+      <c r="B115">
+        <v>2016</v>
+      </c>
+      <c r="C115" t="s">
+        <v>18</v>
+      </c>
+      <c r="D115">
+        <v>13</v>
+      </c>
+      <c r="E115">
+        <v>217</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>127</v>
+      </c>
+      <c r="C2" s="5">
+        <v>636</v>
+      </c>
+      <c r="D2" s="6">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10">
+        <v>25</v>
+      </c>
+      <c r="C3" s="20">
+        <v>-558</v>
+      </c>
+      <c r="D3" s="12">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="10">
+        <v>18</v>
+      </c>
+      <c r="C4" s="11">
+        <v>609</v>
+      </c>
+      <c r="D4" s="12">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>21</v>
+      </c>
+      <c r="C5" s="5">
+        <v>543</v>
+      </c>
+      <c r="D5" s="6">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5">
+        <v>384</v>
+      </c>
+      <c r="D6" s="6">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4">
+        <v>27</v>
+      </c>
+      <c r="C7" s="5">
+        <v>594</v>
+      </c>
+      <c r="D7" s="6">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4">
+        <v>48</v>
+      </c>
+      <c r="C8" s="5">
+        <v>669</v>
+      </c>
+      <c r="D8" s="6">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4">
+        <v>27</v>
+      </c>
+      <c r="C9" s="5">
+        <v>843</v>
+      </c>
+      <c r="D9" s="6">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4">
+        <v>29</v>
+      </c>
+      <c r="C10" s="5">
+        <v>660</v>
+      </c>
+      <c r="D10" s="6">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4">
+        <v>32</v>
+      </c>
+      <c r="C11" s="5">
+        <v>576</v>
+      </c>
+      <c r="D11" s="6">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4">
+        <v>32</v>
+      </c>
+      <c r="C12" s="5">
+        <v>606</v>
+      </c>
+      <c r="D12" s="6">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
+        <v>34</v>
+      </c>
+      <c r="C13" s="5">
+        <v>522</v>
+      </c>
+      <c r="D13" s="6">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4">
+        <v>45</v>
+      </c>
+      <c r="C14" s="5">
+        <v>426</v>
+      </c>
+      <c r="D14" s="6">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4">
+        <v>65</v>
+      </c>
+      <c r="C15" s="5">
+        <v>273</v>
+      </c>
+      <c r="D15" s="6">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4">
+        <v>38</v>
+      </c>
+      <c r="C16" s="5">
+        <v>300</v>
+      </c>
+      <c r="D16" s="6">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4">
+        <v>68</v>
+      </c>
+      <c r="C17" s="5">
+        <v>288</v>
+      </c>
+      <c r="D17" s="6">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4">
+        <v>74</v>
+      </c>
+      <c r="C18" s="5">
+        <v>153</v>
+      </c>
+      <c r="D18" s="6">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4">
+        <v>82</v>
+      </c>
+      <c r="C19" s="5">
+        <v>123</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="4">
+        <v>91</v>
+      </c>
+      <c r="C20" s="5">
+        <v>207</v>
+      </c>
+      <c r="D20" s="6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="14"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
@@ -1824,12 +4113,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40:D58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2655,7 +4944,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
@@ -2957,7 +5246,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -3192,12 +5481,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4028,7 +6317,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
@@ -4564,7 +6853,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
@@ -4875,7 +7164,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
@@ -5331,314 +7620,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4">
-        <v>127</v>
-      </c>
-      <c r="C2" s="5">
-        <v>636</v>
-      </c>
-      <c r="D2" s="6">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="10">
-        <v>25</v>
-      </c>
-      <c r="C3" s="20">
-        <v>-558</v>
-      </c>
-      <c r="D3" s="12">
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="10">
-        <v>18</v>
-      </c>
-      <c r="C4" s="11">
-        <v>609</v>
-      </c>
-      <c r="D4" s="12">
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4">
-        <v>21</v>
-      </c>
-      <c r="C5" s="5">
-        <v>543</v>
-      </c>
-      <c r="D5" s="6">
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4">
-        <v>12</v>
-      </c>
-      <c r="C6" s="5">
-        <v>384</v>
-      </c>
-      <c r="D6" s="6">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4">
-        <v>27</v>
-      </c>
-      <c r="C7" s="5">
-        <v>594</v>
-      </c>
-      <c r="D7" s="6">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4">
-        <v>48</v>
-      </c>
-      <c r="C8" s="5">
-        <v>669</v>
-      </c>
-      <c r="D8" s="6">
-        <v>6500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="4">
-        <v>27</v>
-      </c>
-      <c r="C9" s="5">
-        <v>843</v>
-      </c>
-      <c r="D9" s="6">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="4">
-        <v>29</v>
-      </c>
-      <c r="C10" s="5">
-        <v>660</v>
-      </c>
-      <c r="D10" s="6">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="4">
-        <v>32</v>
-      </c>
-      <c r="C11" s="5">
-        <v>576</v>
-      </c>
-      <c r="D11" s="6">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="4">
-        <v>32</v>
-      </c>
-      <c r="C12" s="5">
-        <v>606</v>
-      </c>
-      <c r="D12" s="6">
-        <v>7000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="4">
-        <v>34</v>
-      </c>
-      <c r="C13" s="5">
-        <v>522</v>
-      </c>
-      <c r="D13" s="6">
-        <v>6500</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="4">
-        <v>45</v>
-      </c>
-      <c r="C14" s="5">
-        <v>426</v>
-      </c>
-      <c r="D14" s="6">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="4">
-        <v>65</v>
-      </c>
-      <c r="C15" s="5">
-        <v>273</v>
-      </c>
-      <c r="D15" s="6">
-        <v>5500</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="4">
-        <v>38</v>
-      </c>
-      <c r="C16" s="5">
-        <v>300</v>
-      </c>
-      <c r="D16" s="6">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="4">
-        <v>68</v>
-      </c>
-      <c r="C17" s="5">
-        <v>288</v>
-      </c>
-      <c r="D17" s="6">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="4">
-        <v>74</v>
-      </c>
-      <c r="C18" s="5">
-        <v>153</v>
-      </c>
-      <c r="D18" s="6">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="4">
-        <v>82</v>
-      </c>
-      <c r="C19" s="5">
-        <v>123</v>
-      </c>
-      <c r="D19" s="6">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="4">
-        <v>91</v>
-      </c>
-      <c r="C20" s="5">
-        <v>207</v>
-      </c>
-      <c r="D20" s="6">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="14"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="15"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Amended DSR test script and Changed DSR output to numerics
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_DSR_ISR_SMR.xlsx
+++ b/tests/testthat/testdata_DSR_ISR_SMR.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="719"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="719" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="testdata_multigroup" sheetId="16" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="58">
   <si>
     <t>0-4</t>
   </si>
@@ -161,9 +161,6 @@
     <t>dsr per 10000</t>
   </si>
   <si>
-    <t>NA - total count is &lt; 10</t>
-  </si>
-  <si>
     <t>observed</t>
   </si>
   <si>
@@ -207,6 +204,9 @@
   </si>
   <si>
     <t>year</t>
+  </si>
+  <si>
+    <t>dsr NA for total count &lt; 10</t>
   </si>
 </sst>
 </file>
@@ -291,7 +291,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -368,6 +368,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -653,7 +659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
@@ -668,7 +674,7 @@
         <v>25</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>26</v>
@@ -2961,10 +2967,10 @@
         <v>21</v>
       </c>
       <c r="E1" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>45</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -4117,8 +4123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4949,7 +4955,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5261,10 +5267,10 @@
         <v>22</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>45</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5485,8 +5491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5504,16 +5510,16 @@
         <v>25</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>44</v>
-      </c>
       <c r="D1" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="17" t="s">
         <v>47</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>48</v>
       </c>
       <c r="F1" s="17" t="s">
         <v>32</v>
@@ -5557,10 +5563,10 @@
         <v>37</v>
       </c>
       <c r="I2" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" t="s">
         <v>49</v>
-      </c>
-      <c r="J2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -5589,10 +5595,10 @@
         <v>37</v>
       </c>
       <c r="I3" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" t="s">
         <v>49</v>
-      </c>
-      <c r="J3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -5621,10 +5627,10 @@
         <v>37</v>
       </c>
       <c r="I4" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -5653,10 +5659,10 @@
         <v>38</v>
       </c>
       <c r="I5" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" t="s">
         <v>49</v>
-      </c>
-      <c r="J5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -5685,10 +5691,10 @@
         <v>38</v>
       </c>
       <c r="I6" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" t="s">
         <v>49</v>
-      </c>
-      <c r="J6" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -5717,10 +5723,10 @@
         <v>38</v>
       </c>
       <c r="I7" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -5753,10 +5759,10 @@
         <v>37</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -5789,10 +5795,10 @@
         <v>37</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -5825,10 +5831,10 @@
         <v>37</v>
       </c>
       <c r="I10" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -5861,10 +5867,10 @@
         <v>38</v>
       </c>
       <c r="I11" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -5897,10 +5903,10 @@
         <v>38</v>
       </c>
       <c r="I12" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -5933,10 +5939,10 @@
         <v>38</v>
       </c>
       <c r="I13" s="25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -5963,10 +5969,10 @@
         <v>37</v>
       </c>
       <c r="I14" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -5993,10 +5999,10 @@
         <v>37</v>
       </c>
       <c r="I15" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -6023,10 +6029,10 @@
         <v>37</v>
       </c>
       <c r="I16" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -6052,10 +6058,10 @@
         <v>38</v>
       </c>
       <c r="I17" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -6081,10 +6087,10 @@
         <v>38</v>
       </c>
       <c r="I18" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -6110,10 +6116,10 @@
         <v>38</v>
       </c>
       <c r="I19" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -6143,10 +6149,10 @@
         <v>37</v>
       </c>
       <c r="I20" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -6176,10 +6182,10 @@
         <v>37</v>
       </c>
       <c r="I21" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -6209,10 +6215,10 @@
         <v>37</v>
       </c>
       <c r="I22" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -6241,10 +6247,10 @@
         <v>38</v>
       </c>
       <c r="I23" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -6273,10 +6279,10 @@
         <v>38</v>
       </c>
       <c r="I24" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -6305,10 +6311,10 @@
         <v>38</v>
       </c>
       <c r="I25" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -6322,7 +6328,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6332,7 +6338,7 @@
     <col min="4" max="4" width="9.140625" style="18"/>
     <col min="5" max="6" width="12" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" style="23" customWidth="1"/>
+    <col min="8" max="8" width="12" style="27" customWidth="1"/>
     <col min="9" max="9" width="11" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6347,7 +6353,7 @@
         <v>28</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>32</v>
@@ -6358,7 +6364,7 @@
       <c r="G1" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="26" t="s">
         <v>39</v>
       </c>
       <c r="I1" s="17" t="s">
@@ -6387,7 +6393,7 @@
       <c r="G2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="27" t="s">
         <v>41</v>
       </c>
       <c r="I2" s="18" t="s">
@@ -6416,7 +6422,7 @@
       <c r="G3" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="27" t="s">
         <v>41</v>
       </c>
       <c r="I3" s="18" t="s">
@@ -6433,20 +6439,11 @@
       <c r="C4">
         <v>8970</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>42</v>
-      </c>
       <c r="G4" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="23" t="s">
-        <v>41</v>
+      <c r="H4" s="27" t="s">
+        <v>57</v>
       </c>
       <c r="I4" s="18" t="s">
         <v>36</v>
@@ -6463,18 +6460,18 @@
         <v>8763</v>
       </c>
       <c r="D5" s="18">
-        <v>8592.0975850223658</v>
+        <v>859.20975850223658</v>
       </c>
       <c r="E5" s="18">
-        <v>7991.160931442103</v>
+        <v>799.11609314421025</v>
       </c>
       <c r="F5" s="18">
-        <v>9225.2538803183179</v>
+        <v>922.52538803183177</v>
       </c>
       <c r="G5" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H5" s="27" t="s">
         <v>41</v>
       </c>
       <c r="I5" s="18" t="s">
@@ -6503,7 +6500,7 @@
       <c r="G6" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="27" t="s">
         <v>41</v>
       </c>
       <c r="I6" s="18" t="s">
@@ -6532,7 +6529,7 @@
       <c r="G7" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="23" t="s">
+      <c r="H7" s="27" t="s">
         <v>41</v>
       </c>
       <c r="I7" s="18" t="s">
@@ -6549,20 +6546,11 @@
       <c r="C8">
         <v>8970</v>
       </c>
-      <c r="D8" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>42</v>
-      </c>
       <c r="G8" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="23" t="s">
-        <v>41</v>
+      <c r="H8" s="27" t="s">
+        <v>57</v>
       </c>
       <c r="I8" s="18" t="s">
         <v>36</v>
@@ -6590,7 +6578,7 @@
       <c r="G9" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="23" t="s">
+      <c r="H9" s="27" t="s">
         <v>41</v>
       </c>
       <c r="I9" s="18" t="s">
@@ -6622,7 +6610,7 @@
       <c r="G10" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="23" t="s">
+      <c r="H10" s="27" t="s">
         <v>40</v>
       </c>
       <c r="I10" s="18" t="s">
@@ -6654,7 +6642,7 @@
       <c r="G11" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="H11" s="27" t="s">
         <v>40</v>
       </c>
       <c r="I11" s="18" t="s">
@@ -6671,20 +6659,11 @@
       <c r="C12">
         <v>8970</v>
       </c>
-      <c r="D12" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>42</v>
-      </c>
       <c r="G12" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="23" t="s">
-        <v>40</v>
+      <c r="H12" s="27" t="s">
+        <v>57</v>
       </c>
       <c r="I12" s="18" t="s">
         <v>36</v>
@@ -6701,21 +6680,18 @@
         <v>8763</v>
       </c>
       <c r="D13" s="18">
-        <f t="shared" ref="D13:F13" si="2">D5*10</f>
-        <v>85920.975850223651</v>
+        <v>8592.0975850223658</v>
       </c>
       <c r="E13" s="18">
-        <f t="shared" si="2"/>
-        <v>79911.609314421032</v>
+        <v>7991.160931442103</v>
       </c>
       <c r="F13" s="18">
-        <f t="shared" si="2"/>
-        <v>92252.538803183183</v>
+        <v>9225.2538803183179</v>
       </c>
       <c r="G13" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="23" t="s">
+      <c r="H13" s="27" t="s">
         <v>40</v>
       </c>
       <c r="I13" s="18" t="s">
@@ -6733,21 +6709,21 @@
         <v>8970</v>
       </c>
       <c r="D14" s="18">
-        <f t="shared" ref="D14:F14" si="3">D6*10</f>
+        <f t="shared" ref="D14:F14" si="2">D6*10</f>
         <v>10430.247991469423</v>
       </c>
       <c r="E14" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>9323.2878802199029</v>
       </c>
       <c r="F14" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>11620.595999522058</v>
       </c>
       <c r="G14" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="23" t="s">
+      <c r="H14" s="27" t="s">
         <v>40</v>
       </c>
       <c r="I14" s="18" t="s">
@@ -6765,21 +6741,21 @@
         <v>8970</v>
       </c>
       <c r="D15" s="18">
-        <f t="shared" ref="D15:F15" si="4">D7*10</f>
+        <f t="shared" ref="D15:F15" si="3">D7*10</f>
         <v>1103.212025300104</v>
       </c>
       <c r="E15" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>763.64203579398793</v>
       </c>
       <c r="F15" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1530.0328948244762</v>
       </c>
       <c r="G15" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H15" s="23" t="s">
+      <c r="H15" s="27" t="s">
         <v>40</v>
       </c>
       <c r="I15" s="18" t="s">
@@ -6796,20 +6772,11 @@
       <c r="C16">
         <v>8970</v>
       </c>
-      <c r="D16" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>42</v>
-      </c>
       <c r="G16" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H16" s="23" t="s">
-        <v>40</v>
+      <c r="H16" s="27" t="s">
+        <v>57</v>
       </c>
       <c r="I16" s="18" t="s">
         <v>36</v>
@@ -6826,21 +6793,21 @@
         <v>8763</v>
       </c>
       <c r="D17" s="18">
-        <f t="shared" ref="D17:F17" si="5">D9*10</f>
+        <f t="shared" ref="D17:F17" si="4">D9*10</f>
         <v>85920.975850223651</v>
       </c>
       <c r="E17" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>76592.821065689554</v>
       </c>
       <c r="F17" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>95992.117985716977</v>
       </c>
       <c r="G17" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="23" t="s">
+      <c r="H17" s="27" t="s">
         <v>40</v>
       </c>
       <c r="I17" s="18" t="s">
@@ -7193,7 +7160,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="4">
         <v>127</v>
@@ -7204,7 +7171,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="10">
         <v>25</v>
@@ -7215,7 +7182,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="10">
         <v>18</v>
@@ -7226,7 +7193,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="4">
         <v>21</v>
@@ -7237,7 +7204,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="4">
         <v>12</v>
@@ -7248,7 +7215,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="4">
         <v>27</v>
@@ -7259,7 +7226,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="4">
         <v>48</v>
@@ -7270,7 +7237,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" s="4">
         <v>27</v>
@@ -7281,7 +7248,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="4">
         <v>29</v>
@@ -7292,7 +7259,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="4">
         <v>32</v>
@@ -7303,7 +7270,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="4">
         <v>32</v>
@@ -7314,7 +7281,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="4">
         <v>34</v>
@@ -7325,7 +7292,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="4">
         <v>45</v>
@@ -7336,7 +7303,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="4">
         <v>65</v>
@@ -7347,7 +7314,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" s="4">
         <v>38</v>
@@ -7358,7 +7325,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="4">
         <v>68</v>
@@ -7369,7 +7336,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" s="4">
         <v>74</v>
@@ -7380,7 +7347,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="4">
         <v>82</v>
@@ -7391,7 +7358,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" s="4">
         <v>91</v>
@@ -7402,7 +7369,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21" s="7">
         <v>12</v>
@@ -7413,7 +7380,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" s="4">
         <v>4</v>
@@ -7424,7 +7391,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" s="4">
         <v>3</v>
@@ -7435,7 +7402,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B24" s="4">
         <v>2</v>
@@ -7446,7 +7413,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" s="4">
         <v>3</v>
@@ -7457,7 +7424,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" s="4">
         <v>4</v>
@@ -7468,7 +7435,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27" s="4">
         <v>8</v>
@@ -7479,7 +7446,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="4">
         <v>2</v>
@@ -7490,7 +7457,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" s="4">
         <v>2</v>
@@ -7501,7 +7468,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B30" s="4">
         <v>3</v>
@@ -7512,7 +7479,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B31" s="4">
         <v>4</v>
@@ -7523,7 +7490,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B32" s="4">
         <v>5</v>
@@ -7534,7 +7501,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B33" s="4">
         <v>6</v>
@@ -7545,7 +7512,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B34" s="4">
         <v>8</v>
@@ -7556,7 +7523,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B35" s="4">
         <v>5</v>
@@ -7567,7 +7534,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B36" s="4">
         <v>6</v>
@@ -7578,7 +7545,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B37" s="4">
         <v>5</v>
@@ -7589,7 +7556,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" s="4">
         <v>5</v>
@@ -7600,7 +7567,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B39" s="4">
         <v>4</v>

</xml_diff>

<commit_message>
Amended DSR function to have stdpoptype = filed or vector parameter. WIP Description updated
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_DSR_ISR_SMR.xlsx
+++ b/tests/testthat/testdata_DSR_ISR_SMR.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="719" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="719" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="testdata_multigroup" sheetId="16" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="59">
   <si>
     <t>0-4</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>dsr NA for total count &lt; 10</t>
+  </si>
+  <si>
+    <t>esp1976</t>
   </si>
 </sst>
 </file>
@@ -4954,8 +4957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4977,7 +4980,7 @@
         <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5491,7 +5494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Amended ISR function and testing so now accepts field name or vector for reference pops.
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_DSR_ISR_SMR.xlsx
+++ b/tests/testthat/testdata_DSR_ISR_SMR.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="719" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="719" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="testdata_multigroup" sheetId="16" r:id="rId1"/>
@@ -294,7 +294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -377,6 +377,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -4127,7 +4137,7 @@
   <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4957,8 +4967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5494,8 +5504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5505,7 +5515,7 @@
     <col min="5" max="6" width="12" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="23" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="23" customWidth="1"/>
-    <col min="9" max="9" width="11" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -5540,471 +5550,445 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2">
+    <row r="2" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="28">
         <v>895</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="28">
         <v>868.50151748646806</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="28">
         <v>9718.074126844951</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="28">
         <v>10014.578176786832</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="28">
         <v>9369.1348126187768</v>
       </c>
-      <c r="G2" s="18">
+      <c r="G2" s="29">
         <v>10692.771133936561</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3">
+    <row r="3" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="28">
         <v>91</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="28">
         <v>868.50151748646806</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="28">
         <v>9718.074126844951</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="28">
         <v>1018.2420269135216</v>
       </c>
-      <c r="F3">
-        <v>819.82496299282775</v>
-      </c>
-      <c r="G3">
-        <v>1250.1755723965371</v>
-      </c>
-      <c r="H3" s="23" t="s">
+      <c r="F3" s="28">
+        <v>819.80264950202934</v>
+      </c>
+      <c r="G3" s="28">
+        <v>1250.1887682774923</v>
+      </c>
+      <c r="H3" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4">
+    <row r="4" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="28">
         <v>9</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="28">
         <v>868.50151748646806</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="28">
         <v>9718.074126844951</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="28">
         <v>100.70525540902962</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="28">
         <v>46.048855430548272</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="29">
         <v>191.16994390980423</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5">
+    <row r="5" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="28">
         <v>895</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="28">
         <v>868.50151748646806</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="28">
         <v>9718.074126844951</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="28">
         <v>10014.578176786832</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="28">
         <v>9011.8539260027446</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="29">
         <v>11092.838181295581</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H5" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6">
+    <row r="6" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="28">
         <v>91</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="28">
         <v>868.50151748646806</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="28">
         <v>9718.074126844951</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="28">
         <v>1018.2420269135216</v>
       </c>
-      <c r="F6">
-        <v>719.96754227969689</v>
-      </c>
-      <c r="G6">
-        <v>1393.1902906954499</v>
-      </c>
-      <c r="H6" s="23" t="s">
+      <c r="F6" s="28">
+        <v>719.76056742794265</v>
+      </c>
+      <c r="G6" s="28">
+        <v>1393.4168657142982</v>
+      </c>
+      <c r="H6" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7">
+    <row r="7" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="28">
         <v>9</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="28">
         <v>868.50151748646806</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="28">
         <v>9718.074126844951</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="28">
         <v>100.70525540902962</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="28">
         <v>27.441336223643425</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="28">
         <v>253.52406288743475</v>
       </c>
-      <c r="H7" s="23" t="s">
+      <c r="H7" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8">
+    <row r="8" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="28">
         <v>895</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="28">
         <v>868.50151748646806</v>
       </c>
-      <c r="D8">
-        <f>D2/100</f>
+      <c r="D8" s="28">
         <v>97.180741268449509</v>
       </c>
-      <c r="E8">
-        <f t="shared" ref="E8:G8" si="0">E2/100</f>
+      <c r="E8" s="28">
         <v>100.14578176786831</v>
       </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
+      <c r="F8" s="28">
         <v>93.691348126187762</v>
       </c>
-      <c r="G8">
-        <f t="shared" si="0"/>
+      <c r="G8" s="28">
         <v>106.92771133936562</v>
       </c>
-      <c r="H8" s="23" t="s">
+      <c r="H8" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9">
+    <row r="9" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="28">
         <v>91</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="28">
         <v>868.50151748646806</v>
       </c>
-      <c r="D9">
-        <f t="shared" ref="D9:G9" si="1">D3/100</f>
+      <c r="D9" s="28">
         <v>97.180741268449509</v>
       </c>
-      <c r="E9">
-        <f t="shared" si="1"/>
+      <c r="E9" s="28">
         <v>10.182420269135216</v>
       </c>
-      <c r="F9">
-        <f t="shared" si="1"/>
-        <v>8.1982496299282772</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="1"/>
-        <v>12.50175572396537</v>
-      </c>
-      <c r="H9" s="23" t="s">
+      <c r="F9" s="28">
+        <v>8.1980264950202937</v>
+      </c>
+      <c r="G9" s="28">
+        <v>12.501887682774923</v>
+      </c>
+      <c r="H9" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="25" t="s">
+      <c r="I9" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10">
+    <row r="10" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="28">
         <v>9</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="28">
         <v>868.50151748646806</v>
       </c>
-      <c r="D10">
-        <f t="shared" ref="D10:G10" si="2">D4/100</f>
+      <c r="D10" s="28">
         <v>97.180741268449509</v>
       </c>
-      <c r="E10">
-        <f t="shared" si="2"/>
+      <c r="E10" s="28">
         <v>1.0070525540902961</v>
       </c>
-      <c r="F10">
-        <f t="shared" si="2"/>
+      <c r="F10" s="28">
         <v>0.46048855430548274</v>
       </c>
-      <c r="G10">
-        <f t="shared" si="2"/>
+      <c r="G10" s="28">
         <v>1.9116994390980424</v>
       </c>
-      <c r="H10" s="23" t="s">
+      <c r="H10" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="25" t="s">
+      <c r="I10" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11">
+    <row r="11" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="28">
         <v>895</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="28">
         <v>868.50151748646806</v>
       </c>
-      <c r="D11">
-        <f t="shared" ref="D11:G11" si="3">D5/100</f>
+      <c r="D11" s="28">
         <v>97.180741268449509</v>
       </c>
-      <c r="E11">
-        <f t="shared" si="3"/>
+      <c r="E11" s="28">
         <v>100.14578176786831</v>
       </c>
-      <c r="F11">
-        <f t="shared" si="3"/>
+      <c r="F11" s="28">
         <v>90.118539260027447</v>
       </c>
-      <c r="G11">
-        <f t="shared" si="3"/>
+      <c r="G11" s="28">
         <v>110.92838181295582</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="H11" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="25" t="s">
+      <c r="I11" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12">
+    <row r="12" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="28">
         <v>91</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="28">
         <v>868.50151748646806</v>
       </c>
-      <c r="D12">
-        <f t="shared" ref="D12:G12" si="4">D6/100</f>
+      <c r="D12" s="28">
         <v>97.180741268449509</v>
       </c>
-      <c r="E12">
-        <f t="shared" si="4"/>
+      <c r="E12" s="28">
         <v>10.182420269135216</v>
       </c>
-      <c r="F12">
-        <f t="shared" si="4"/>
-        <v>7.199675422796969</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="4"/>
-        <v>13.931902906954498</v>
-      </c>
-      <c r="H12" s="23" t="s">
+      <c r="F12" s="28">
+        <v>7.1976056742794263</v>
+      </c>
+      <c r="G12" s="28">
+        <v>13.934168657142981</v>
+      </c>
+      <c r="H12" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="25" t="s">
+      <c r="I12" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13">
+    <row r="13" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="28">
         <v>9</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="28">
         <v>868.50151748646806</v>
       </c>
-      <c r="D13">
-        <f t="shared" ref="D13:G13" si="5">D7/100</f>
+      <c r="D13" s="28">
         <v>97.180741268449509</v>
       </c>
-      <c r="E13">
-        <f t="shared" si="5"/>
+      <c r="E13" s="28">
         <v>1.0070525540902961</v>
       </c>
-      <c r="F13">
-        <f t="shared" si="5"/>
+      <c r="F13" s="28">
         <v>0.27441336223643426</v>
       </c>
-      <c r="G13">
-        <f t="shared" si="5"/>
+      <c r="G13" s="28">
         <v>2.5352406288743476</v>
       </c>
-      <c r="H13" s="23" t="s">
+      <c r="H13" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="I13" s="25" t="s">
+      <c r="I13" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14">
+    <row r="14" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="28">
         <v>895</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="28">
         <v>868.50151748646806</v>
       </c>
-      <c r="D14"/>
-      <c r="E14">
+      <c r="E14" s="28">
         <v>1.030510577103217</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="28">
         <v>0.96409377931556683</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="28">
         <v>1.1002973422891613</v>
       </c>
-      <c r="H14" s="23" t="s">
+      <c r="H14" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="I14" s="25" t="s">
+      <c r="I14" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15">
+    <row r="15" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="28">
         <v>91</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="28">
         <v>868.50151748646806</v>
       </c>
-      <c r="D15"/>
-      <c r="E15" s="18">
+      <c r="E15" s="29">
         <v>0.10477817040937738</v>
       </c>
-      <c r="F15" s="18">
-        <v>8.4360846839824463E-2</v>
-      </c>
-      <c r="G15" s="23">
-        <v>0.12864437501491011</v>
-      </c>
-      <c r="H15" s="23" t="s">
+      <c r="F15" s="29">
+        <v>8.4358550758264761E-2</v>
+      </c>
+      <c r="G15" s="30">
+        <v>0.12864573288487313</v>
+      </c>
+      <c r="H15" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="I15" s="25" t="s">
+      <c r="I15" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="28" t="s">
         <v>49</v>
       </c>
     </row>
@@ -6081,10 +6065,10 @@
         <v>0.10477817040937738</v>
       </c>
       <c r="F18" s="18">
-        <v>7.4085413723165336E-2</v>
+        <v>7.4064115794269886E-2</v>
       </c>
       <c r="G18" s="23">
-        <v>0.14336073922784123</v>
+        <v>0.14338405403444704</v>
       </c>
       <c r="H18" s="23" t="s">
         <v>38</v>
@@ -6137,15 +6121,12 @@
       </c>
       <c r="D20"/>
       <c r="E20">
-        <f>E14*100</f>
         <v>103.0510577103217</v>
       </c>
       <c r="F20">
-        <f t="shared" ref="F20:G20" si="6">F14*100</f>
         <v>96.409377931556691</v>
       </c>
       <c r="G20">
-        <f t="shared" si="6"/>
         <v>110.02973422891613</v>
       </c>
       <c r="H20" s="23" t="s">
@@ -6170,16 +6151,13 @@
       </c>
       <c r="D21"/>
       <c r="E21">
-        <f t="shared" ref="E21:G21" si="7">E15*100</f>
         <v>10.477817040937738</v>
       </c>
       <c r="F21">
-        <f t="shared" si="7"/>
-        <v>8.4360846839824468</v>
+        <v>8.4358550758264759</v>
       </c>
       <c r="G21">
-        <f t="shared" si="7"/>
-        <v>12.864437501491011</v>
+        <v>12.864573288487314</v>
       </c>
       <c r="H21" s="23" t="s">
         <v>37</v>
@@ -6203,15 +6181,12 @@
       </c>
       <c r="D22"/>
       <c r="E22">
-        <f t="shared" ref="E22:G22" si="8">E16*100</f>
         <v>1.0362676194334028</v>
       </c>
       <c r="F22">
-        <f t="shared" si="8"/>
         <v>0.47384754252227951</v>
       </c>
       <c r="G22">
-        <f t="shared" si="8"/>
         <v>1.9671587334544141</v>
       </c>
       <c r="H22" s="23" t="s">
@@ -6235,15 +6210,12 @@
         <v>868.50151748646806</v>
       </c>
       <c r="E23">
-        <f t="shared" ref="E23:G23" si="9">E17*100</f>
         <v>103.0510577103217</v>
       </c>
       <c r="F23">
-        <f t="shared" si="9"/>
         <v>92.73292021007164</v>
       </c>
       <c r="G23">
-        <f t="shared" si="9"/>
         <v>114.14646602306746</v>
       </c>
       <c r="H23" s="23" t="s">
@@ -6267,16 +6239,13 @@
         <v>868.50151748646806</v>
       </c>
       <c r="E24">
-        <f t="shared" ref="E24:G24" si="10">E18*100</f>
         <v>10.477817040937738</v>
       </c>
       <c r="F24">
-        <f t="shared" si="10"/>
-        <v>7.4085413723165336</v>
+        <v>7.4064115794269885</v>
       </c>
       <c r="G24">
-        <f t="shared" si="10"/>
-        <v>14.336073922784124</v>
+        <v>14.338405403444703</v>
       </c>
       <c r="H24" s="23" t="s">
         <v>38</v>
@@ -6299,15 +6268,12 @@
         <v>868.50151748646806</v>
       </c>
       <c r="E25">
-        <f t="shared" ref="E25:G25" si="11">E19*100</f>
         <v>1.0362676194334028</v>
       </c>
       <c r="F25">
-        <f t="shared" si="11"/>
         <v>0.2823742221500472</v>
       </c>
       <c r="G25">
-        <f t="shared" si="11"/>
         <v>2.6087891446218401</v>
       </c>
       <c r="H25" s="23" t="s">

</xml_diff>

<commit_message>
Amended ISR and SMR so work with age specific denominators of 0. Amended testthat scripts accordingly.
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_DSR_ISR_SMR.xlsx
+++ b/tests/testthat/testdata_DSR_ISR_SMR.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="59">
   <si>
     <t>0-4</t>
   </si>
@@ -294,7 +294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -388,6 +388,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5502,10 +5505,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6284,6 +6287,128 @@
       </c>
       <c r="J25" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="32">
+        <v>895</v>
+      </c>
+      <c r="C26" s="32">
+        <v>840.93969634711902</v>
+      </c>
+      <c r="D26" s="32">
+        <v>9718.074126844951</v>
+      </c>
+      <c r="E26" s="32">
+        <v>10342.806245569416</v>
+      </c>
+      <c r="F26" s="32">
+        <v>9676.2084578011254</v>
+      </c>
+      <c r="G26" s="32">
+        <v>11043.22699510916</v>
+      </c>
+      <c r="H26" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="J26" s="25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27">
+        <v>91</v>
+      </c>
+      <c r="C27" s="18">
+        <v>868.50151748646806</v>
+      </c>
+      <c r="D27" s="18">
+        <v>9718.074126844951</v>
+      </c>
+      <c r="E27" s="18">
+        <v>1018.2420269135216</v>
+      </c>
+      <c r="F27" s="18">
+        <v>819.80264950202934</v>
+      </c>
+      <c r="G27" s="23">
+        <v>1250.1887682774923</v>
+      </c>
+      <c r="H27" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I27" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="J27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28">
+        <v>895</v>
+      </c>
+      <c r="C28" s="18">
+        <v>840.93969634711902</v>
+      </c>
+      <c r="E28" s="18">
+        <v>106.42855889521074</v>
+      </c>
+      <c r="F28" s="18">
+        <v>99.569197883270135</v>
+      </c>
+      <c r="G28" s="23">
+        <v>113.63596172418198</v>
+      </c>
+      <c r="H28" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I28" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="J28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29">
+        <v>91</v>
+      </c>
+      <c r="C29" s="18">
+        <v>868.50151748646806</v>
+      </c>
+      <c r="E29" s="18">
+        <v>10.477817040937738</v>
+      </c>
+      <c r="F29" s="18">
+        <v>8.4358550758264759</v>
+      </c>
+      <c r="G29" s="23">
+        <v>12.864573288487314</v>
+      </c>
+      <c r="H29" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I29" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="J29" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed coding to allow functions to run with NA input values and compute results where appropriate.  Need to complete ISr and SMR testdata with NA values.
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_DSR_ISR_SMR.xlsx
+++ b/tests/testthat/testdata_DSR_ISR_SMR.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Georgina.Anderson\Documents\R\Projects\PHEstatmethods\tests\testthat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georgina.anderson\Documents\R\Projects\PHEindicatormethods\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCE3ACD-0621-46F6-8530-AD1600CF861D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="719" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="719" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata_multigroup" sheetId="16" r:id="rId1"/>
@@ -23,10 +24,16 @@
     <sheet name="testdata_err2" sheetId="8" r:id="rId9"/>
     <sheet name="testdata_err3" sheetId="9" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -215,7 +222,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="??0.00"/>
     <numFmt numFmtId="165" formatCode="?,??0"/>
@@ -395,7 +402,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -672,11 +679,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2647,11 +2654,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2957,11 +2964,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4136,11 +4143,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4729,9 +4736,6 @@
       <c r="B42" t="s">
         <v>2</v>
       </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
       <c r="D42">
         <v>609</v>
       </c>
@@ -4967,11 +4971,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5269,7 +5273,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5504,11 +5508,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6418,11 +6422,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6915,7 +6919,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7226,7 +7230,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
All NA handling and test scripts complete for dsr, isr and smr functions.
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_DSR_ISR_SMR.xlsx
+++ b/tests/testthat/testdata_DSR_ISR_SMR.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georgina.anderson\Documents\R\Projects\PHEindicatormethods\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCE3ACD-0621-46F6-8530-AD1600CF861D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F49F87-280A-4CD4-A151-20946C22F0EF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="719" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="719" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata_multigroup" sheetId="16" r:id="rId1"/>
-    <sheet name="testdata_multiarea_ref" sheetId="15" r:id="rId2"/>
+    <sheet name="testdata_multiarea_isrsmr" sheetId="15" r:id="rId2"/>
     <sheet name="testdata_multiarea" sheetId="5" r:id="rId3"/>
     <sheet name="testdata_1976" sheetId="12" r:id="rId4"/>
     <sheet name="refdata" sheetId="14" r:id="rId5"/>
@@ -229,7 +229,7 @@
     <numFmt numFmtId="166" formatCode="??,??0"/>
     <numFmt numFmtId="167" formatCode="?,???,??0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,6 +273,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -301,7 +315,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -374,29 +388,44 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -682,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E115"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G128" sqref="G128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2967,8 +2996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3050,7 +3079,7 @@
         <v>609</v>
       </c>
       <c r="E4">
-        <v>3225</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>60213</v>
@@ -3430,7 +3459,7 @@
         <v>609</v>
       </c>
       <c r="E23">
-        <v>3225</v>
+        <v>0</v>
       </c>
       <c r="F23">
         <v>60213</v>
@@ -3802,15 +3831,6 @@
       </c>
       <c r="B42" t="s">
         <v>2</v>
-      </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="D42">
-        <v>609</v>
-      </c>
-      <c r="E42">
-        <v>3225</v>
       </c>
       <c r="F42">
         <v>60213</v>
@@ -4146,8 +4166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4975,7 +4995,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5269,20 +5289,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>22</v>
       </c>
@@ -5292,8 +5313,9 @@
       <c r="C1" s="16" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5304,7 +5326,7 @@
         <v>50520</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -5315,18 +5337,18 @@
         <v>57173</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>3225</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>60213</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -5337,7 +5359,7 @@
         <v>54659</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -5348,7 +5370,7 @@
         <v>44345</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -5359,7 +5381,7 @@
         <v>50128</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -5370,7 +5392,7 @@
         <v>62163</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -5381,7 +5403,7 @@
         <v>67423</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -5392,7 +5414,7 @@
         <v>62899</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -5403,7 +5425,7 @@
         <v>55463</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -5414,7 +5436,7 @@
         <v>60479</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -5425,7 +5447,7 @@
         <v>49974</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -5436,7 +5458,7 @@
         <v>44140</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -5447,7 +5469,7 @@
         <v>40888</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -5511,8 +5533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5521,8 +5543,9 @@
     <col min="3" max="4" width="9.140625" style="18"/>
     <col min="5" max="6" width="12" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" style="23" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="25" customWidth="1"/>
+    <col min="8" max="8" width="12" style="34" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="35" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -5547,871 +5570,877 @@
       <c r="G1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="30" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="28">
+    <row r="2" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="33">
         <v>895</v>
       </c>
-      <c r="C2" s="28">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="D2" s="28">
-        <v>9718.074126844951</v>
-      </c>
-      <c r="E2" s="28">
-        <v>10014.578176786832</v>
-      </c>
-      <c r="F2" s="28">
-        <v>9369.1348126187768</v>
-      </c>
-      <c r="G2" s="29">
-        <v>10692.771133936561</v>
-      </c>
-      <c r="H2" s="30" t="s">
+      <c r="C2" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="D2" s="33">
+        <v>9349.8830922110192</v>
+      </c>
+      <c r="E2" s="33">
+        <v>10011.137622091057</v>
+      </c>
+      <c r="F2" s="33">
+        <v>9365.91600297888</v>
+      </c>
+      <c r="G2" s="37">
+        <v>10689.097582910616</v>
+      </c>
+      <c r="H2" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="28">
+    <row r="3" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="33">
         <v>91</v>
       </c>
-      <c r="C3" s="28">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="D3" s="28">
-        <v>9718.074126844951</v>
-      </c>
-      <c r="E3" s="28">
-        <v>1018.2420269135216</v>
-      </c>
-      <c r="F3" s="28">
-        <v>819.80264950202934</v>
-      </c>
-      <c r="G3" s="28">
-        <v>1250.1887682774923</v>
-      </c>
-      <c r="H3" s="30" t="s">
+      <c r="C3" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="D3" s="33">
+        <v>9349.8830922110192</v>
+      </c>
+      <c r="E3" s="33">
+        <v>1017.8922051511577</v>
+      </c>
+      <c r="F3" s="33">
+        <v>819.52100250646299</v>
+      </c>
+      <c r="G3" s="33">
+        <v>1249.7592601383201</v>
+      </c>
+      <c r="H3" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="31" t="s">
+      <c r="I3" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="28" t="s">
+      <c r="J3" s="33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="28">
+    <row r="4" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="33">
         <v>9</v>
       </c>
-      <c r="C4" s="28">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="D4" s="28">
-        <v>9718.074126844951</v>
-      </c>
-      <c r="E4" s="28">
-        <v>100.70525540902962</v>
-      </c>
-      <c r="F4" s="28">
-        <v>46.048855430548272</v>
-      </c>
-      <c r="G4" s="29">
-        <v>191.16994390980423</v>
-      </c>
-      <c r="H4" s="30" t="s">
+      <c r="C4" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="D4" s="33">
+        <v>9349.8830922110192</v>
+      </c>
+      <c r="E4" s="33">
+        <v>100.6706576523123</v>
+      </c>
+      <c r="F4" s="33">
+        <v>46.033035133078933</v>
+      </c>
+      <c r="G4" s="37">
+        <v>191.10426659054028</v>
+      </c>
+      <c r="H4" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="31" t="s">
+      <c r="I4" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="33" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="28">
+    <row r="5" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="33">
         <v>895</v>
       </c>
-      <c r="C5" s="28">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="D5" s="28">
-        <v>9718.074126844951</v>
-      </c>
-      <c r="E5" s="28">
-        <v>10014.578176786832</v>
-      </c>
-      <c r="F5" s="28">
-        <v>9011.8539260027446</v>
-      </c>
-      <c r="G5" s="29">
-        <v>11092.838181295581</v>
-      </c>
-      <c r="H5" s="30" t="s">
+      <c r="C5" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="D5" s="33">
+        <v>9349.8830922110192</v>
+      </c>
+      <c r="E5" s="33">
+        <v>10011.137622091057</v>
+      </c>
+      <c r="F5" s="33">
+        <v>9008.7578618655007</v>
+      </c>
+      <c r="G5" s="37">
+        <v>11089.02718538338</v>
+      </c>
+      <c r="H5" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="J5" s="28" t="s">
+      <c r="J5" s="33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="28">
+    <row r="6" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="33">
         <v>91</v>
       </c>
-      <c r="C6" s="28">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="D6" s="28">
-        <v>9718.074126844951</v>
-      </c>
-      <c r="E6" s="28">
-        <v>1018.2420269135216</v>
-      </c>
-      <c r="F6" s="28">
-        <v>719.76056742794265</v>
-      </c>
-      <c r="G6" s="28">
-        <v>1393.4168657142982</v>
-      </c>
-      <c r="H6" s="30" t="s">
+      <c r="C6" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="D6" s="33">
+        <v>9349.8830922110192</v>
+      </c>
+      <c r="E6" s="33">
+        <v>1017.8922051511577</v>
+      </c>
+      <c r="F6" s="33">
+        <v>719.51329035282447</v>
+      </c>
+      <c r="G6" s="33">
+        <v>1392.9381508991678</v>
+      </c>
+      <c r="H6" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="J6" s="28" t="s">
+      <c r="J6" s="33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="28">
+    <row r="7" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="33">
         <v>9</v>
       </c>
-      <c r="C7" s="28">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="D7" s="28">
-        <v>9718.074126844951</v>
-      </c>
-      <c r="E7" s="28">
-        <v>100.70525540902962</v>
-      </c>
-      <c r="F7" s="28">
-        <v>27.441336223643425</v>
-      </c>
-      <c r="G7" s="28">
-        <v>253.52406288743475</v>
-      </c>
-      <c r="H7" s="30" t="s">
+      <c r="C7" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="D7" s="33">
+        <v>9349.8830922110192</v>
+      </c>
+      <c r="E7" s="33">
+        <v>100.6706576523123</v>
+      </c>
+      <c r="F7" s="33">
+        <v>27.431908625542341</v>
+      </c>
+      <c r="G7" s="33">
+        <v>253.43696352192359</v>
+      </c>
+      <c r="H7" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="31" t="s">
+      <c r="I7" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="28" t="s">
+      <c r="J7" s="33" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="28">
+    <row r="8" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="33">
         <v>895</v>
       </c>
-      <c r="C8" s="28">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="D8" s="28">
-        <v>97.180741268449509</v>
-      </c>
-      <c r="E8" s="28">
-        <v>100.14578176786831</v>
-      </c>
-      <c r="F8" s="28">
-        <v>93.691348126187762</v>
-      </c>
-      <c r="G8" s="28">
-        <v>106.92771133936562</v>
-      </c>
-      <c r="H8" s="30" t="s">
+      <c r="C8" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="D8" s="33">
+        <v>93.498830922110187</v>
+      </c>
+      <c r="E8" s="33">
+        <v>100.11137622091056</v>
+      </c>
+      <c r="F8" s="33">
+        <v>93.659160029788794</v>
+      </c>
+      <c r="G8" s="33">
+        <v>106.89097582910615</v>
+      </c>
+      <c r="H8" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="31" t="s">
+      <c r="I8" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="J8" s="28" t="s">
+      <c r="J8" s="33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="28">
+    <row r="9" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="33">
         <v>91</v>
       </c>
-      <c r="C9" s="28">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="D9" s="28">
-        <v>97.180741268449509</v>
-      </c>
-      <c r="E9" s="28">
-        <v>10.182420269135216</v>
-      </c>
-      <c r="F9" s="28">
-        <v>8.1980264950202937</v>
-      </c>
-      <c r="G9" s="28">
-        <v>12.501887682774923</v>
-      </c>
-      <c r="H9" s="30" t="s">
+      <c r="C9" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="D9" s="33">
+        <v>93.498830922110187</v>
+      </c>
+      <c r="E9" s="33">
+        <v>10.178922051511577</v>
+      </c>
+      <c r="F9" s="33">
+        <v>8.1952100250646307</v>
+      </c>
+      <c r="G9" s="33">
+        <v>12.497592601383202</v>
+      </c>
+      <c r="H9" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="31" t="s">
+      <c r="I9" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="J9" s="28" t="s">
+      <c r="J9" s="33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="28">
+    <row r="10" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="33">
         <v>9</v>
       </c>
-      <c r="C10" s="28">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="D10" s="28">
-        <v>97.180741268449509</v>
-      </c>
-      <c r="E10" s="28">
-        <v>1.0070525540902961</v>
-      </c>
-      <c r="F10" s="28">
-        <v>0.46048855430548274</v>
-      </c>
-      <c r="G10" s="28">
-        <v>1.9116994390980424</v>
-      </c>
-      <c r="H10" s="30" t="s">
+      <c r="C10" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="D10" s="33">
+        <v>93.498830922110187</v>
+      </c>
+      <c r="E10" s="33">
+        <v>1.0067065765231229</v>
+      </c>
+      <c r="F10" s="33">
+        <v>0.46033035133078931</v>
+      </c>
+      <c r="G10" s="33">
+        <v>1.9110426659054027</v>
+      </c>
+      <c r="H10" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="31" t="s">
+      <c r="I10" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="J10" s="28" t="s">
+      <c r="J10" s="33" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="28">
+    <row r="11" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="33">
         <v>895</v>
       </c>
-      <c r="C11" s="28">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="D11" s="28">
-        <v>97.180741268449509</v>
-      </c>
-      <c r="E11" s="28">
-        <v>100.14578176786831</v>
-      </c>
-      <c r="F11" s="28">
-        <v>90.118539260027447</v>
-      </c>
-      <c r="G11" s="28">
-        <v>110.92838181295582</v>
-      </c>
-      <c r="H11" s="30" t="s">
+      <c r="C11" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="D11" s="33">
+        <v>93.498830922110187</v>
+      </c>
+      <c r="E11" s="33">
+        <v>100.11137622091056</v>
+      </c>
+      <c r="F11" s="33">
+        <v>90.087578618655002</v>
+      </c>
+      <c r="G11" s="33">
+        <v>110.8902718538338</v>
+      </c>
+      <c r="H11" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="J11" s="28" t="s">
+      <c r="J11" s="33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="28">
+    <row r="12" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="33">
         <v>91</v>
       </c>
-      <c r="C12" s="28">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="D12" s="28">
-        <v>97.180741268449509</v>
-      </c>
-      <c r="E12" s="28">
-        <v>10.182420269135216</v>
-      </c>
-      <c r="F12" s="28">
-        <v>7.1976056742794263</v>
-      </c>
-      <c r="G12" s="28">
-        <v>13.934168657142981</v>
-      </c>
-      <c r="H12" s="30" t="s">
+      <c r="C12" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="D12" s="33">
+        <v>93.498830922110187</v>
+      </c>
+      <c r="E12" s="33">
+        <v>10.178922051511577</v>
+      </c>
+      <c r="F12" s="33">
+        <v>7.1951329035282443</v>
+      </c>
+      <c r="G12" s="33">
+        <v>13.929381508991677</v>
+      </c>
+      <c r="H12" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="31" t="s">
+      <c r="I12" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="J12" s="28" t="s">
+      <c r="J12" s="33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="28">
+    <row r="13" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="33">
         <v>9</v>
       </c>
-      <c r="C13" s="28">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="D13" s="28">
-        <v>97.180741268449509</v>
-      </c>
-      <c r="E13" s="28">
-        <v>1.0070525540902961</v>
-      </c>
-      <c r="F13" s="28">
-        <v>0.27441336223643426</v>
-      </c>
-      <c r="G13" s="28">
-        <v>2.5352406288743476</v>
-      </c>
-      <c r="H13" s="30" t="s">
+      <c r="C13" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="D13" s="33">
+        <v>93.498830922110187</v>
+      </c>
+      <c r="E13" s="33">
+        <v>1.0067065765231229</v>
+      </c>
+      <c r="F13" s="33">
+        <v>0.27431908625542339</v>
+      </c>
+      <c r="G13" s="33">
+        <v>2.5343696352192358</v>
+      </c>
+      <c r="H13" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="I13" s="31" t="s">
+      <c r="I13" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="J13" s="28" t="s">
+      <c r="J13" s="33" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="28">
+    <row r="14" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="33">
         <v>895</v>
       </c>
-      <c r="C14" s="28">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="E14" s="28">
-        <v>1.030510577103217</v>
-      </c>
-      <c r="F14" s="28">
-        <v>0.96409377931556683</v>
-      </c>
-      <c r="G14" s="28">
-        <v>1.1002973422891613</v>
-      </c>
-      <c r="H14" s="30" t="s">
+      <c r="C14" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="E14" s="33">
+        <v>1.0707232939020275</v>
+      </c>
+      <c r="F14" s="33">
+        <v>1.0017147712553987</v>
+      </c>
+      <c r="G14" s="33">
+        <v>1.1432332872498949</v>
+      </c>
+      <c r="H14" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="I14" s="31" t="s">
+      <c r="I14" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="J14" s="28" t="s">
+      <c r="J14" s="33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="28">
+    <row r="15" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="33">
         <v>91</v>
       </c>
-      <c r="C15" s="28">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="E15" s="29">
-        <v>0.10477817040937738</v>
-      </c>
-      <c r="F15" s="29">
-        <v>8.4358550758264761E-2</v>
-      </c>
-      <c r="G15" s="30">
-        <v>0.12864573288487313</v>
-      </c>
-      <c r="H15" s="30" t="s">
+      <c r="C15" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="E15" s="37">
+        <v>0.10886683770400503</v>
+      </c>
+      <c r="F15" s="37">
+        <v>8.765040101829405E-2</v>
+      </c>
+      <c r="G15" s="31">
+        <v>0.13366576328418911</v>
+      </c>
+      <c r="H15" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="I15" s="31" t="s">
+      <c r="I15" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="J15" s="28" t="s">
+      <c r="J15" s="33" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16">
+    <row r="16" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="36">
         <v>9</v>
       </c>
-      <c r="C16">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="D16"/>
-      <c r="E16" s="18">
-        <v>1.0362676194334028E-2</v>
-      </c>
-      <c r="F16" s="18">
-        <v>4.7384754252227951E-3</v>
-      </c>
-      <c r="G16" s="18">
-        <v>1.967158733454414E-2</v>
-      </c>
-      <c r="H16" s="23" t="s">
+      <c r="C16" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="D16" s="36"/>
+      <c r="E16" s="38">
+        <v>1.0767049882813684E-2</v>
+      </c>
+      <c r="F16" s="38">
+        <v>4.9233808250957762E-3</v>
+      </c>
+      <c r="G16" s="38">
+        <v>2.043921455549973E-2</v>
+      </c>
+      <c r="H16" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="I16" s="25" t="s">
+      <c r="I16" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J16" s="36" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17">
+    <row r="17" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="36">
         <v>895</v>
       </c>
-      <c r="C17" s="18">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="E17">
-        <v>1.030510577103217</v>
-      </c>
-      <c r="F17">
-        <v>0.92732920210071634</v>
-      </c>
-      <c r="G17" s="18">
-        <v>1.1414646602306746</v>
-      </c>
-      <c r="H17" s="23" t="s">
+      <c r="C17" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="D17" s="38"/>
+      <c r="E17" s="36">
+        <v>1.0707232939020275</v>
+      </c>
+      <c r="F17" s="36">
+        <v>0.96351556196144372</v>
+      </c>
+      <c r="G17" s="38">
+        <v>1.1860070415876287</v>
+      </c>
+      <c r="H17" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="I17" s="25" t="s">
+      <c r="I17" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J17" s="36" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18">
+    <row r="18" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="36">
         <v>91</v>
       </c>
-      <c r="C18" s="18">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="E18" s="18">
-        <v>0.10477817040937738</v>
-      </c>
-      <c r="F18" s="18">
-        <v>7.4064115794269886E-2</v>
-      </c>
-      <c r="G18" s="23">
-        <v>0.14338405403444704</v>
-      </c>
-      <c r="H18" s="23" t="s">
+      <c r="C18" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38">
+        <v>0.10886683770400503</v>
+      </c>
+      <c r="F18" s="38">
+        <v>7.6954255283921108E-2</v>
+      </c>
+      <c r="G18" s="34">
+        <v>0.14897920510466744</v>
+      </c>
+      <c r="H18" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="I18" s="25" t="s">
+      <c r="I18" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="36" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19">
+    <row r="19" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="36">
         <v>9</v>
       </c>
-      <c r="C19" s="18">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="E19" s="18">
-        <v>1.0362676194334028E-2</v>
-      </c>
-      <c r="F19" s="18">
-        <v>2.8237422215004722E-3</v>
-      </c>
-      <c r="G19" s="23">
-        <v>2.6087891446218401E-2</v>
-      </c>
-      <c r="H19" s="23" t="s">
+      <c r="C19" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38">
+        <v>1.0767049882813684E-2</v>
+      </c>
+      <c r="F19" s="38">
+        <v>2.9339306550682617E-3</v>
+      </c>
+      <c r="G19" s="34">
+        <v>2.7105896514690211E-2</v>
+      </c>
+      <c r="H19" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="I19" s="25" t="s">
+      <c r="I19" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="36" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20">
+    <row r="20" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="36">
         <v>895</v>
       </c>
-      <c r="C20">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="D20"/>
-      <c r="E20">
-        <v>103.0510577103217</v>
-      </c>
-      <c r="F20">
-        <v>96.409377931556691</v>
-      </c>
-      <c r="G20">
-        <v>110.02973422891613</v>
-      </c>
-      <c r="H20" s="23" t="s">
+      <c r="C20" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="E20" s="36">
+        <v>107.07232939020275</v>
+      </c>
+      <c r="F20" s="36">
+        <v>100.17147712553987</v>
+      </c>
+      <c r="G20" s="36">
+        <v>114.32332872498949</v>
+      </c>
+      <c r="H20" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="I20" s="25" t="s">
+      <c r="I20" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="36" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21">
+    <row r="21" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="36">
         <v>91</v>
       </c>
-      <c r="C21">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="D21"/>
-      <c r="E21">
-        <v>10.477817040937738</v>
-      </c>
-      <c r="F21">
-        <v>8.4358550758264759</v>
-      </c>
-      <c r="G21">
-        <v>12.864573288487314</v>
-      </c>
-      <c r="H21" s="23" t="s">
+      <c r="C21" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="E21" s="36">
+        <v>10.886683770400502</v>
+      </c>
+      <c r="F21" s="36">
+        <v>8.7650401018294044</v>
+      </c>
+      <c r="G21" s="36">
+        <v>13.366576328418912</v>
+      </c>
+      <c r="H21" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="I21" s="25" t="s">
+      <c r="I21" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J21" s="36" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22">
+    <row r="22" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="36">
         <v>9</v>
       </c>
-      <c r="C22">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="D22"/>
-      <c r="E22">
-        <v>1.0362676194334028</v>
-      </c>
-      <c r="F22">
-        <v>0.47384754252227951</v>
-      </c>
-      <c r="G22">
-        <v>1.9671587334544141</v>
-      </c>
-      <c r="H22" s="23" t="s">
+      <c r="C22" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36">
+        <v>1.0767049882813684</v>
+      </c>
+      <c r="F22" s="36">
+        <v>0.49233808250957761</v>
+      </c>
+      <c r="G22" s="36">
+        <v>2.043921455549973</v>
+      </c>
+      <c r="H22" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="I22" s="25" t="s">
+      <c r="I22" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J22" s="36" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23">
+    <row r="23" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="36">
         <v>895</v>
       </c>
-      <c r="C23" s="18">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="E23">
-        <v>103.0510577103217</v>
-      </c>
-      <c r="F23">
-        <v>92.73292021007164</v>
-      </c>
-      <c r="G23">
-        <v>114.14646602306746</v>
-      </c>
-      <c r="H23" s="23" t="s">
+      <c r="C23" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="D23" s="38"/>
+      <c r="E23" s="36">
+        <v>107.07232939020275</v>
+      </c>
+      <c r="F23" s="36">
+        <v>96.351556196144372</v>
+      </c>
+      <c r="G23" s="36">
+        <v>118.60070415876287</v>
+      </c>
+      <c r="H23" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="I23" s="25" t="s">
+      <c r="I23" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="36" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24">
+    <row r="24" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="36">
         <v>91</v>
       </c>
-      <c r="C24" s="18">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="E24">
-        <v>10.477817040937738</v>
-      </c>
-      <c r="F24">
-        <v>7.4064115794269885</v>
-      </c>
-      <c r="G24">
-        <v>14.338405403444703</v>
-      </c>
-      <c r="H24" s="23" t="s">
+      <c r="C24" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="D24" s="38"/>
+      <c r="E24" s="36">
+        <v>10.886683770400502</v>
+      </c>
+      <c r="F24" s="36">
+        <v>7.6954255283921107</v>
+      </c>
+      <c r="G24" s="36">
+        <v>14.897920510466744</v>
+      </c>
+      <c r="H24" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="I24" s="25" t="s">
+      <c r="I24" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" s="36" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25">
+    <row r="25" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="36">
         <v>9</v>
       </c>
-      <c r="C25" s="18">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="E25">
-        <v>1.0362676194334028</v>
-      </c>
-      <c r="F25">
-        <v>0.2823742221500472</v>
-      </c>
-      <c r="G25">
-        <v>2.6087891446218401</v>
-      </c>
-      <c r="H25" s="23" t="s">
+      <c r="C25" s="33">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="D25" s="38"/>
+      <c r="E25" s="36">
+        <v>1.0767049882813684</v>
+      </c>
+      <c r="F25" s="36">
+        <v>0.2933930655068262</v>
+      </c>
+      <c r="G25" s="36">
+        <v>2.7105896514690211</v>
+      </c>
+      <c r="H25" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="I25" s="25" t="s">
+      <c r="I25" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="36" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="32">
+      <c r="B26" s="39">
         <v>895</v>
       </c>
-      <c r="C26" s="32">
-        <v>840.93969634711902</v>
-      </c>
-      <c r="D26" s="32">
-        <v>9718.074126844951</v>
-      </c>
-      <c r="E26" s="32">
-        <v>10342.806245569416</v>
-      </c>
-      <c r="F26" s="32">
-        <v>9676.2084578011254</v>
-      </c>
-      <c r="G26" s="32">
-        <v>11043.22699510916</v>
-      </c>
-      <c r="H26" s="23" t="s">
+      <c r="C26" s="39">
+        <v>808.32174009182529</v>
+      </c>
+      <c r="D26" s="39">
+        <v>9349.8830922110192</v>
+      </c>
+      <c r="E26" s="39">
+        <v>10352.493261629017</v>
+      </c>
+      <c r="F26" s="39">
+        <v>9685.2711419993229</v>
+      </c>
+      <c r="G26" s="39">
+        <v>11053.570021432142</v>
+      </c>
+      <c r="H26" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="I26" s="25" t="s">
+      <c r="I26" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="J26" s="25" t="s">
+      <c r="J26" s="35" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="36">
         <v>91</v>
       </c>
-      <c r="C27" s="18">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="D27" s="18">
-        <v>9718.074126844951</v>
-      </c>
-      <c r="E27" s="18">
-        <v>1018.2420269135216</v>
-      </c>
-      <c r="F27" s="18">
-        <v>819.80264950202934</v>
-      </c>
-      <c r="G27" s="23">
-        <v>1250.1887682774923</v>
-      </c>
-      <c r="H27" s="23" t="s">
+      <c r="C27" s="38">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="D27" s="38">
+        <v>9349.8830922110192</v>
+      </c>
+      <c r="E27" s="38">
+        <v>1017.8922051511577</v>
+      </c>
+      <c r="F27" s="38">
+        <v>819.52100250646299</v>
+      </c>
+      <c r="G27" s="34">
+        <v>1249.7592601383201</v>
+      </c>
+      <c r="H27" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="I27" s="25" t="s">
+      <c r="I27" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27" s="36" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="36">
         <v>895</v>
       </c>
-      <c r="C28" s="18">
-        <v>840.93969634711902</v>
-      </c>
-      <c r="E28" s="18">
-        <v>106.42855889521074</v>
-      </c>
-      <c r="F28" s="18">
-        <v>99.569197883270135</v>
-      </c>
-      <c r="G28" s="23">
-        <v>113.63596172418198</v>
-      </c>
-      <c r="H28" s="23" t="s">
+      <c r="C28" s="38">
+        <v>808.32174009182529</v>
+      </c>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38">
+        <v>110.72323749430866</v>
+      </c>
+      <c r="F28" s="38">
+        <v>103.58708281676485</v>
+      </c>
+      <c r="G28" s="34">
+        <v>118.22147841228508</v>
+      </c>
+      <c r="H28" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="I28" s="25" t="s">
+      <c r="I28" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J28" s="36" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="36">
         <v>91</v>
       </c>
-      <c r="C29" s="18">
-        <v>868.50151748646806</v>
-      </c>
-      <c r="E29" s="18">
-        <v>10.477817040937738</v>
-      </c>
-      <c r="F29" s="18">
-        <v>8.4358550758264759</v>
-      </c>
-      <c r="G29" s="23">
-        <v>12.864573288487314</v>
-      </c>
-      <c r="H29" s="23" t="s">
+      <c r="C29" s="38">
+        <v>835.88356123117433</v>
+      </c>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38">
+        <v>10.886683770400502</v>
+      </c>
+      <c r="F29" s="38">
+        <v>8.7650401018294044</v>
+      </c>
+      <c r="G29" s="34">
+        <v>13.366576328418912</v>
+      </c>
+      <c r="H29" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="I29" s="25" t="s">
+      <c r="I29" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J29" s="36" t="s">
         <v>49</v>
       </c>
     </row>
@@ -6436,7 +6465,7 @@
     <col min="4" max="4" width="9.140625" style="18"/>
     <col min="5" max="6" width="12" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" style="27" customWidth="1"/>
+    <col min="8" max="8" width="12" style="25" customWidth="1"/>
     <col min="9" max="9" width="11" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6462,7 +6491,7 @@
       <c r="G1" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="24" t="s">
         <v>39</v>
       </c>
       <c r="I1" s="17" t="s">
@@ -6491,7 +6520,7 @@
       <c r="G2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="25" t="s">
         <v>41</v>
       </c>
       <c r="I2" s="18" t="s">
@@ -6520,7 +6549,7 @@
       <c r="G3" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="25" t="s">
         <v>41</v>
       </c>
       <c r="I3" s="18" t="s">
@@ -6540,7 +6569,7 @@
       <c r="G4" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="25" t="s">
         <v>57</v>
       </c>
       <c r="I4" s="18" t="s">
@@ -6569,7 +6598,7 @@
       <c r="G5" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="H5" s="25" t="s">
         <v>41</v>
       </c>
       <c r="I5" s="18" t="s">
@@ -6598,7 +6627,7 @@
       <c r="G6" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="25" t="s">
         <v>41</v>
       </c>
       <c r="I6" s="18" t="s">
@@ -6627,7 +6656,7 @@
       <c r="G7" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="27" t="s">
+      <c r="H7" s="25" t="s">
         <v>41</v>
       </c>
       <c r="I7" s="18" t="s">
@@ -6647,7 +6676,7 @@
       <c r="G8" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="25" t="s">
         <v>57</v>
       </c>
       <c r="I8" s="18" t="s">
@@ -6676,7 +6705,7 @@
       <c r="G9" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="27" t="s">
+      <c r="H9" s="25" t="s">
         <v>41</v>
       </c>
       <c r="I9" s="18" t="s">
@@ -6708,7 +6737,7 @@
       <c r="G10" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="27" t="s">
+      <c r="H10" s="25" t="s">
         <v>40</v>
       </c>
       <c r="I10" s="18" t="s">
@@ -6740,7 +6769,7 @@
       <c r="G11" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="27" t="s">
+      <c r="H11" s="25" t="s">
         <v>40</v>
       </c>
       <c r="I11" s="18" t="s">
@@ -6760,7 +6789,7 @@
       <c r="G12" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="H12" s="25" t="s">
         <v>57</v>
       </c>
       <c r="I12" s="18" t="s">
@@ -6789,7 +6818,7 @@
       <c r="G13" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="27" t="s">
+      <c r="H13" s="25" t="s">
         <v>40</v>
       </c>
       <c r="I13" s="18" t="s">
@@ -6821,7 +6850,7 @@
       <c r="G14" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="27" t="s">
+      <c r="H14" s="25" t="s">
         <v>40</v>
       </c>
       <c r="I14" s="18" t="s">
@@ -6853,7 +6882,7 @@
       <c r="G15" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H15" s="27" t="s">
+      <c r="H15" s="25" t="s">
         <v>40</v>
       </c>
       <c r="I15" s="18" t="s">
@@ -6873,7 +6902,7 @@
       <c r="G16" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H16" s="27" t="s">
+      <c r="H16" s="25" t="s">
         <v>57</v>
       </c>
       <c r="I16" s="18" t="s">
@@ -6905,7 +6934,7 @@
       <c r="G17" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="27" t="s">
+      <c r="H17" s="25" t="s">
         <v>40</v>
       </c>
       <c r="I17" s="18" t="s">
@@ -7233,8 +7262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Amended test data and scripts to include new standardised_pop output field for DSRs.
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_DSR_ISR_SMR.xlsx
+++ b/tests/testthat/testdata_DSR_ISR_SMR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georgina.anderson\Documents\R\Projects\PHEindicatormethods\tests\testthat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Georgina.Anderson\Documents\R\Projects\PHEindicatormethods\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F49F87-280A-4CD4-A151-20946C22F0EF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{751F8A65-6B7C-42EF-B524-46B091ED7A90}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="719" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="719" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata_multigroup" sheetId="16" r:id="rId1"/>
@@ -24,23 +24,17 @@
     <sheet name="testdata_err2" sheetId="8" r:id="rId9"/>
     <sheet name="testdata_err3" sheetId="9" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="60">
   <si>
     <t>0-4</t>
   </si>
@@ -217,6 +211,9 @@
   </si>
   <si>
     <t>esp1976</t>
+  </si>
+  <si>
+    <t>standardised_pop</t>
   </si>
 </sst>
 </file>
@@ -2996,7 +2993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21:D39"/>
     </sheetView>
   </sheetViews>
@@ -4166,8 +4163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40:D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4995,7 +4992,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D2" sqref="D2:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5533,8 +5530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6452,24 +6449,25 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="18"/>
-    <col min="5" max="6" width="12" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" style="25" customWidth="1"/>
-    <col min="9" max="9" width="11" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="18"/>
+    <col min="6" max="7" width="12" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="25" customWidth="1"/>
+    <col min="10" max="10" width="11" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>25</v>
       </c>
@@ -6479,26 +6477,29 @@
       <c r="C1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="H1" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="I1" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="J1" s="17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -6508,26 +6509,29 @@
       <c r="C2">
         <v>8970</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2">
+        <v>10430.247991469423</v>
+      </c>
+      <c r="E2" s="18">
         <v>1043.0247991469423</v>
       </c>
-      <c r="E2" s="18">
+      <c r="F2" s="18">
         <v>971.77090679856803</v>
       </c>
-      <c r="F2" s="18">
+      <c r="G2" s="18">
         <v>1117.894091547925</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="H2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="I2" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="J2" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -6537,26 +6541,29 @@
       <c r="C3">
         <v>8970</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3">
+        <v>1103.212025300104</v>
+      </c>
+      <c r="E3" s="18">
         <v>110.3212025300104</v>
       </c>
-      <c r="E3" s="18">
+      <c r="F3" s="18">
         <v>87.745576753670903</v>
       </c>
-      <c r="F3" s="18">
+      <c r="G3" s="18">
         <v>136.70882227251795</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="H3" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="I3" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="J3" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -6566,17 +6573,17 @@
       <c r="C4">
         <v>8970</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="H4" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="I4" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="J4" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -6586,26 +6593,29 @@
       <c r="C5">
         <v>8763</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5">
+        <v>8592.0975850223658</v>
+      </c>
+      <c r="E5" s="18">
         <v>859.20975850223658</v>
       </c>
-      <c r="E5" s="18">
+      <c r="F5" s="18">
         <v>799.11609314421025</v>
       </c>
-      <c r="F5" s="18">
+      <c r="G5" s="18">
         <v>922.52538803183177</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="H5" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="I5" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="J5" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -6615,26 +6625,29 @@
       <c r="C6">
         <v>8970</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6">
+        <v>10430.247991469423</v>
+      </c>
+      <c r="E6" s="18">
         <v>1043.0247991469423</v>
       </c>
-      <c r="E6" s="18">
+      <c r="F6" s="18">
         <v>932.32878802199036</v>
       </c>
-      <c r="F6" s="18">
+      <c r="G6" s="18">
         <v>1162.0595999522059</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="H6" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="I6" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="J6" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -6644,26 +6657,29 @@
       <c r="C7">
         <v>8970</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7">
+        <v>1103.212025300104</v>
+      </c>
+      <c r="E7" s="18">
         <v>110.3212025300104</v>
       </c>
-      <c r="E7" s="18">
+      <c r="F7" s="18">
         <v>76.36420357939879</v>
       </c>
-      <c r="F7" s="18">
+      <c r="G7" s="18">
         <v>153.00328948244763</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="H7" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="I7" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="J7" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -6673,17 +6689,17 @@
       <c r="C8">
         <v>8970</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="H8" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="I8" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="J8" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -6693,26 +6709,29 @@
       <c r="C9">
         <v>8763</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9">
         <v>8592.0975850223658</v>
       </c>
       <c r="E9" s="18">
+        <v>8592.0975850223658</v>
+      </c>
+      <c r="F9" s="18">
         <v>7659.2821065689559</v>
       </c>
-      <c r="F9" s="18">
+      <c r="G9" s="18">
         <v>9599.2117985716977</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="H9" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="I9" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="J9" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -6722,29 +6741,32 @@
       <c r="C10">
         <v>8970</v>
       </c>
-      <c r="D10" s="18">
-        <f>D2*10</f>
+      <c r="D10">
         <v>10430.247991469423</v>
       </c>
       <c r="E10" s="18">
-        <f t="shared" ref="E10:F10" si="0">E2*10</f>
+        <f>E2*10</f>
+        <v>10430.247991469423</v>
+      </c>
+      <c r="F10" s="18">
+        <f t="shared" ref="F10:G10" si="0">F2*10</f>
         <v>9717.709067985681</v>
       </c>
-      <c r="F10" s="18">
+      <c r="G10" s="18">
         <f t="shared" si="0"/>
         <v>11178.94091547925</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="H10" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="I10" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="18" t="s">
+      <c r="J10" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -6754,29 +6776,32 @@
       <c r="C11">
         <v>8970</v>
       </c>
-      <c r="D11" s="18">
-        <f t="shared" ref="D11:F11" si="1">D3*10</f>
+      <c r="D11">
         <v>1103.212025300104</v>
       </c>
       <c r="E11" s="18">
+        <f t="shared" ref="E11:G11" si="1">E3*10</f>
+        <v>1103.212025300104</v>
+      </c>
+      <c r="F11" s="18">
         <f t="shared" si="1"/>
         <v>877.455767536709</v>
       </c>
-      <c r="F11" s="18">
+      <c r="G11" s="18">
         <f t="shared" si="1"/>
         <v>1367.0882227251795</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="H11" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="I11" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="I11" s="18" t="s">
+      <c r="J11" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -6786,17 +6811,17 @@
       <c r="C12">
         <v>8970</v>
       </c>
-      <c r="G12" s="23" t="s">
+      <c r="H12" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="25" t="s">
+      <c r="I12" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="I12" s="18" t="s">
+      <c r="J12" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -6806,26 +6831,29 @@
       <c r="C13">
         <v>8763</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13">
         <v>8592.0975850223658</v>
       </c>
       <c r="E13" s="18">
+        <v>8592.0975850223658</v>
+      </c>
+      <c r="F13" s="18">
         <v>7991.160931442103</v>
       </c>
-      <c r="F13" s="18">
+      <c r="G13" s="18">
         <v>9225.2538803183179</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="H13" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="I13" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="I13" s="18" t="s">
+      <c r="J13" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -6835,29 +6863,32 @@
       <c r="C14">
         <v>8970</v>
       </c>
-      <c r="D14" s="18">
-        <f t="shared" ref="D14:F14" si="2">D6*10</f>
+      <c r="D14">
         <v>10430.247991469423</v>
       </c>
       <c r="E14" s="18">
+        <f t="shared" ref="E14:G14" si="2">E6*10</f>
+        <v>10430.247991469423</v>
+      </c>
+      <c r="F14" s="18">
         <f t="shared" si="2"/>
         <v>9323.2878802199029</v>
       </c>
-      <c r="F14" s="18">
+      <c r="G14" s="18">
         <f t="shared" si="2"/>
         <v>11620.595999522058</v>
       </c>
-      <c r="G14" s="23" t="s">
+      <c r="H14" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="25" t="s">
+      <c r="I14" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="I14" s="18" t="s">
+      <c r="J14" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -6867,29 +6898,32 @@
       <c r="C15">
         <v>8970</v>
       </c>
-      <c r="D15" s="18">
-        <f t="shared" ref="D15:F15" si="3">D7*10</f>
+      <c r="D15">
         <v>1103.212025300104</v>
       </c>
       <c r="E15" s="18">
+        <f t="shared" ref="E15:G15" si="3">E7*10</f>
+        <v>1103.212025300104</v>
+      </c>
+      <c r="F15" s="18">
         <f t="shared" si="3"/>
         <v>763.64203579398793</v>
       </c>
-      <c r="F15" s="18">
+      <c r="G15" s="18">
         <f t="shared" si="3"/>
         <v>1530.0328948244762</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="H15" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H15" s="25" t="s">
+      <c r="I15" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="I15" s="18" t="s">
+      <c r="J15" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -6899,17 +6933,17 @@
       <c r="C16">
         <v>8970</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="H16" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H16" s="25" t="s">
+      <c r="I16" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="I16" s="18" t="s">
+      <c r="J16" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -6919,25 +6953,28 @@
       <c r="C17">
         <v>8763</v>
       </c>
-      <c r="D17" s="18">
-        <f t="shared" ref="D17:F17" si="4">D9*10</f>
+      <c r="D17">
+        <v>8592.0975850223658</v>
+      </c>
+      <c r="E17" s="18">
+        <f t="shared" ref="E17:G17" si="4">E9*10</f>
         <v>85920.975850223651</v>
       </c>
-      <c r="E17" s="18">
+      <c r="F17" s="18">
         <f t="shared" si="4"/>
         <v>76592.821065689554</v>
       </c>
-      <c r="F17" s="18">
+      <c r="G17" s="18">
         <f t="shared" si="4"/>
         <v>95992.117985716977</v>
       </c>
-      <c r="G17" s="23" t="s">
+      <c r="H17" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="25" t="s">
+      <c r="I17" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="I17" s="18" t="s">
+      <c r="J17" s="18" t="s">
         <v>36</v>
       </c>
     </row>
@@ -7262,7 +7299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21:C39"/>
     </sheetView>
   </sheetViews>

</xml_diff>